<commit_message>
KMP001_Update Update Print Master
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMP001.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMP001.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B41331A1-6E0C-42DD-94F7-8B1E44C4446B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="3525" windowWidth="29100" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10710"/>
   </bookViews>
   <sheets>
     <sheet name="KMP001" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>【会社】</t>
     <rPh sb="1" eb="3">
@@ -65,18 +64,52 @@
   <si>
     <t>有効桁数</t>
   </si>
+  <si>
+    <t>【sheet名】</t>
+  </si>
+  <si>
+    <t>マスタリスト</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Meiryo UI"/>
+      <family val="2"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,8 +144,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -122,8 +166,13 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="標準 10" xfId="3"/>
+    <cellStyle name="標準 2" xfId="2"/>
+    <cellStyle name="標準 3" xfId="1"/>
+    <cellStyle name="標準 3 10" xfId="4"/>
+    <cellStyle name="標準 3 2 8" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -400,20 +449,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -421,7 +470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -429,7 +478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -437,12 +486,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -450,13 +502,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
KMP001 FIx bug 123695
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMP001.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMP001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10710"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="10725"/>
   </bookViews>
   <sheets>
     <sheet name="マスタリスト" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>【会社】</t>
     <rPh sb="1" eb="3">
@@ -29,9 +29,6 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
-    <t>01　日通システム株式会社</t>
-  </si>
-  <si>
     <t>【種類】</t>
     <rPh sb="1" eb="3">
       <t>シュルイ</t>
@@ -39,9 +36,6 @@
     <phoneticPr fontId="0"/>
   </si>
   <si>
-    <t>KMP001_カードNOの登録</t>
-  </si>
-  <si>
     <t>【日時】</t>
     <rPh sb="1" eb="3">
       <t>ニチジ</t>
@@ -69,6 +63,9 @@
   </si>
   <si>
     <t>マスタリスト</t>
+  </si>
+  <si>
+    <t>KMP001_打刻カードの設定</t>
   </si>
 </sst>
 </file>
@@ -453,7 +450,7 @@
   <dimension ref="A3:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -466,51 +463,48 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B14" s="3"/>
     </row>

</xml_diff>